<commit_message>
update to r4 qa
</commit_message>
<xml_diff>
--- a/source/resources/source-data/DEQM_Capability_Statement_Consumer_Client.xlsx
+++ b/source/resources/source-data/DEQM_Capability_Statement_Consumer_Client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-DEQM\source\resources\source-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF6BD67-F1FD-415E-B648-1D348F5E24E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7ED1E5-23AF-403B-BA29-039D5E65BDE7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="1" activeTab="4" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -225,49 +225,25 @@
     <t>For general security consideration refer to the [Security and Privacy Considerations](http://build.fhir.org/secpriv-module.html).</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/STU3/StructureDefinition/devicerequest-deqm</t>
-  </si>
-  <si>
     <t>DeviceRequest</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/STU3/StructureDefinition/medicationadministration-deqm</t>
-  </si>
-  <si>
     <t>MedicationAdministration</t>
   </si>
   <si>
     <t>MeasureReport</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/STU3/StructureDefinition/datax-measurereport-deqm</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/STU3/StructureDefinition/practitioner-deqm</t>
-  </si>
-  <si>
     <t>Practitioner</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/STU3/StructureDefinition/deviceusestatement-deqm</t>
-  </si>
-  <si>
     <t>DeviceUseStatement</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/STU3/StructureDefinition/organization-deqm</t>
-  </si>
-  <si>
     <t>Organization</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/STU3/StructureDefinition/coverage-deqm</t>
-  </si>
-  <si>
     <t>Coverage</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/STU3/StructureDefinition/medicationrequest-deqm</t>
   </si>
   <si>
     <t>MedicationRequest</t>
@@ -338,18 +314,9 @@
     <t>version</t>
   </si>
   <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
     <t>fhirVersion</t>
   </si>
   <si>
-    <t>3.0.1</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/ImplementationGuide/hl7.fhir.us.davinci-deqm-1.0.0</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/qicore/ImplementationGuide/us-qicore-3.2.0</t>
   </si>
   <si>
@@ -471,6 +438,39 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/OperationDefinition/Measure-collect-data</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-deqm/StructureDefinition/devicerequest-deqm</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-deqm/StructureDefinition/datax-measurereport-deqm</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-deqm/StructureDefinition/medicationadministration-deqm</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-deqm/StructureDefinition/practitioner-deqm</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-deqm/StructureDefinition/deviceusestatement-deqm</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-deqm/StructureDefinition/organization-deqm</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-deqm/StructureDefinition/coverage-deqm</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-deqm/StructureDefinition/medicationrequest-deqm</t>
+  </si>
+  <si>
+    <t>4.0.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-deqm/ImplementationGuide/hl7.fhir.us.davinci-deqm-1.1.0</t>
   </si>
 </sst>
 </file>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15F3286-55C1-40D0-93FC-C97EF26956B8}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,18 +933,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -952,7 +952,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -960,7 +960,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -968,7 +968,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>89</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -976,7 +976,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -984,7 +984,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1019,23 +1019,23 @@
         <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1049,7 +1049,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,128 +1076,128 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" t="s">
         <v>63</v>
-      </c>
-      <c r="B9" t="s">
-        <v>71</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1245,61 +1245,61 @@
         <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F1" t="s">
         <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="H1" t="s">
         <v>37</v>
       </c>
       <c r="I1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="J1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="K1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="L1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="M1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="N1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="O1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="P1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="Q1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="R1" t="s">
         <v>27</v>
       </c>
       <c r="S1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="W1" s="7" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="X1" t="s">
         <v>47</v>
@@ -1307,27 +1307,27 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1347,8 +1347,8 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,16 +1379,16 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1420,10 +1420,10 @@
         <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1441,10 +1441,10 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1504,42 +1504,42 @@
         <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -1643,34 +1643,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1678,20 +1678,20 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="J2" s="8" t="str">
         <f t="shared" ref="J2" si="1">"Fetches a bundle of all "&amp;B2&amp;" resources matching the specified "&amp;SUBSTITUTE(D2,","," and ")</f>

</xml_diff>